<commit_message>
Site updated: 2026-02-27 03:50:19
</commit_message>
<xml_diff>
--- a/AxB_Nasal/resources/conditions.xlsx
+++ b/AxB_Nasal/resources/conditions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luoziwei/Desktop/psychopy script/AXB_Madarian Nasal ai/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luoziwei/Desktop/psychopy script/AXB_Madarian Nasal ai/html/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0380F146-E886-F44C-AD4F-96CAEF7EC99D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE8DFC1-B4A0-8847-9F6D-9F79766226D0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="620" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="259" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="259" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>